<commit_message>
Grade Card Updated v2
Grade Card Updated v2
</commit_message>
<xml_diff>
--- a/Backup/Grade Card - Backup.xlsx
+++ b/Backup/Grade Card - Backup.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abhishek Chitnis\Videos\Results Genetaor\Batch 2018-20\Sem 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\AutoMBA\Results Genetaor\Batch 2018-20\Sem 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C0A915-37F9-4CD2-B573-7C154D007FA5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D70EB4-3B72-4023-BFE5-62958018F6AC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4C80AD8E-6BB5-43FA-A2DF-2A6A1A9D1C00}"/>
   </bookViews>
@@ -176,7 +176,7 @@
     <t>DECEMBER 2018</t>
   </si>
   <si>
-    <t>MMS18-20/20</t>
+    <t>MMS18-20/1</t>
   </si>
 </sst>
 </file>
@@ -504,20 +504,20 @@
           <xdr:col>16</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>19049</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>17</xdr:col>
           <xdr:colOff>828675</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>180975</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="8" name="Picture 7">
+            <xdr:cNvPr id="5" name="Picture 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C8854B5-4655-43C8-8E81-122493EAE494}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23A67F1B-C1FA-4994-8EC0-9370F76DEED6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -525,7 +525,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="PicUp" spid="_x0000_s2098"/>
+                  <a14:cameraTool cellRange="PicUp" spid="_x0000_s2112"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -539,8 +539,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="7353300" y="1295399"/>
-              <a:ext cx="1181100" cy="1047751"/>
+              <a:off x="7353300" y="1304925"/>
+              <a:ext cx="1181100" cy="1028700"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1901,6 +1901,110 @@
             <v>NA</v>
           </cell>
         </row>
+        <row r="122">
+          <cell r="A122" t="str">
+            <v>MMS18-20/121</v>
+          </cell>
+          <cell r="B122" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="123">
+          <cell r="A123" t="str">
+            <v>MMS18-20/122</v>
+          </cell>
+          <cell r="B123" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="124">
+          <cell r="A124" t="str">
+            <v>MMS18-20/123</v>
+          </cell>
+          <cell r="B124" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="125">
+          <cell r="A125" t="str">
+            <v>MMS18-20/124</v>
+          </cell>
+          <cell r="B125" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="126">
+          <cell r="A126" t="str">
+            <v>MMS18-20/125</v>
+          </cell>
+          <cell r="B126" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="127">
+          <cell r="A127" t="str">
+            <v>MMS18-20/126</v>
+          </cell>
+          <cell r="B127" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="128">
+          <cell r="A128" t="str">
+            <v>MMS18-20/127</v>
+          </cell>
+          <cell r="B128" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="129">
+          <cell r="A129" t="str">
+            <v>MMS18-20/128</v>
+          </cell>
+          <cell r="B129" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="130">
+          <cell r="A130" t="str">
+            <v>MMS18-20/129</v>
+          </cell>
+          <cell r="B130" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="131">
+          <cell r="A131" t="str">
+            <v>MMS18-20/130</v>
+          </cell>
+          <cell r="B131" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="132">
+          <cell r="A132" t="str">
+            <v>MMS18-20/131</v>
+          </cell>
+          <cell r="B132" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="133">
+          <cell r="A133" t="str">
+            <v>MMS18-20/132</v>
+          </cell>
+          <cell r="B133" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
+        <row r="134">
+          <cell r="A134" t="str">
+            <v>MMS18-20/133</v>
+          </cell>
+          <cell r="B134" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+        </row>
       </sheetData>
     </sheetDataSet>
   </externalBook>
@@ -26633,6 +26737,2216 @@
           </cell>
           <cell r="BP122" t="str">
             <v>65-69.99</v>
+          </cell>
+        </row>
+        <row r="123">
+          <cell r="A123" t="str">
+            <v>MMS18-20/121</v>
+          </cell>
+          <cell r="B123" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+          <cell r="C123">
+            <v>0</v>
+          </cell>
+          <cell r="D123">
+            <v>0</v>
+          </cell>
+          <cell r="E123">
+            <v>0</v>
+          </cell>
+          <cell r="F123" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="G123" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="H123">
+            <v>4</v>
+          </cell>
+          <cell r="I123">
+            <v>0</v>
+          </cell>
+          <cell r="J123">
+            <v>0</v>
+          </cell>
+          <cell r="K123">
+            <v>0</v>
+          </cell>
+          <cell r="L123">
+            <v>0</v>
+          </cell>
+          <cell r="M123" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="N123" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="O123">
+            <v>4</v>
+          </cell>
+          <cell r="P123">
+            <v>0</v>
+          </cell>
+          <cell r="Q123">
+            <v>0</v>
+          </cell>
+          <cell r="R123">
+            <v>0</v>
+          </cell>
+          <cell r="S123">
+            <v>0</v>
+          </cell>
+          <cell r="T123" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="U123" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="V123">
+            <v>4</v>
+          </cell>
+          <cell r="W123">
+            <v>0</v>
+          </cell>
+          <cell r="X123">
+            <v>28</v>
+          </cell>
+          <cell r="Y123">
+            <v>37</v>
+          </cell>
+          <cell r="Z123">
+            <v>65</v>
+          </cell>
+          <cell r="AA123" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="AB123" t="str">
+            <v>7</v>
+          </cell>
+          <cell r="AC123">
+            <v>4</v>
+          </cell>
+          <cell r="AD123">
+            <v>28</v>
+          </cell>
+          <cell r="AE123">
+            <v>28</v>
+          </cell>
+          <cell r="AF123">
+            <v>37</v>
+          </cell>
+          <cell r="AG123">
+            <v>65</v>
+          </cell>
+          <cell r="AH123" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="AI123" t="str">
+            <v>7</v>
+          </cell>
+          <cell r="AJ123">
+            <v>4</v>
+          </cell>
+          <cell r="AK123">
+            <v>28</v>
+          </cell>
+          <cell r="AL123">
+            <v>28</v>
+          </cell>
+          <cell r="AM123">
+            <v>37</v>
+          </cell>
+          <cell r="AN123">
+            <v>65</v>
+          </cell>
+          <cell r="AO123" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="AP123" t="str">
+            <v>7</v>
+          </cell>
+          <cell r="AQ123">
+            <v>4</v>
+          </cell>
+          <cell r="AR123">
+            <v>28</v>
+          </cell>
+          <cell r="AS123">
+            <v>28</v>
+          </cell>
+          <cell r="AT123">
+            <v>37</v>
+          </cell>
+          <cell r="AU123">
+            <v>65</v>
+          </cell>
+          <cell r="AV123" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="AW123" t="str">
+            <v>7</v>
+          </cell>
+          <cell r="AX123">
+            <v>4</v>
+          </cell>
+          <cell r="AY123">
+            <v>28</v>
+          </cell>
+          <cell r="AZ123">
+            <v>28</v>
+          </cell>
+          <cell r="BA123">
+            <v>37</v>
+          </cell>
+          <cell r="BB123">
+            <v>65</v>
+          </cell>
+          <cell r="BC123" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="BD123" t="str">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="124">
+          <cell r="A124" t="str">
+            <v>MMS18-20/122</v>
+          </cell>
+          <cell r="B124" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+          <cell r="C124">
+            <v>0</v>
+          </cell>
+          <cell r="D124">
+            <v>0</v>
+          </cell>
+          <cell r="E124">
+            <v>0</v>
+          </cell>
+          <cell r="F124" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="G124" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="H124">
+            <v>4</v>
+          </cell>
+          <cell r="I124">
+            <v>0</v>
+          </cell>
+          <cell r="J124">
+            <v>0</v>
+          </cell>
+          <cell r="K124">
+            <v>0</v>
+          </cell>
+          <cell r="L124">
+            <v>0</v>
+          </cell>
+          <cell r="M124" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="N124" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="O124">
+            <v>4</v>
+          </cell>
+          <cell r="P124">
+            <v>0</v>
+          </cell>
+          <cell r="Q124">
+            <v>0</v>
+          </cell>
+          <cell r="R124">
+            <v>0</v>
+          </cell>
+          <cell r="S124">
+            <v>0</v>
+          </cell>
+          <cell r="T124" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="U124" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="V124">
+            <v>4</v>
+          </cell>
+          <cell r="W124">
+            <v>0</v>
+          </cell>
+          <cell r="X124">
+            <v>30</v>
+          </cell>
+          <cell r="Y124">
+            <v>40</v>
+          </cell>
+          <cell r="Z124">
+            <v>70</v>
+          </cell>
+          <cell r="AA124" t="str">
+            <v>A</v>
+          </cell>
+          <cell r="AB124" t="str">
+            <v>8</v>
+          </cell>
+          <cell r="AC124">
+            <v>4</v>
+          </cell>
+          <cell r="AD124">
+            <v>32</v>
+          </cell>
+          <cell r="AE124">
+            <v>30</v>
+          </cell>
+          <cell r="AF124">
+            <v>40</v>
+          </cell>
+          <cell r="AG124">
+            <v>70</v>
+          </cell>
+          <cell r="AH124" t="str">
+            <v>A</v>
+          </cell>
+          <cell r="AI124" t="str">
+            <v>8</v>
+          </cell>
+          <cell r="AJ124">
+            <v>4</v>
+          </cell>
+          <cell r="AK124">
+            <v>32</v>
+          </cell>
+          <cell r="AL124">
+            <v>30</v>
+          </cell>
+          <cell r="AM124">
+            <v>40</v>
+          </cell>
+          <cell r="AN124">
+            <v>70</v>
+          </cell>
+          <cell r="AO124" t="str">
+            <v>A</v>
+          </cell>
+          <cell r="AP124" t="str">
+            <v>8</v>
+          </cell>
+          <cell r="AQ124">
+            <v>4</v>
+          </cell>
+          <cell r="AR124">
+            <v>32</v>
+          </cell>
+          <cell r="AS124">
+            <v>30</v>
+          </cell>
+          <cell r="AT124">
+            <v>40</v>
+          </cell>
+          <cell r="AU124">
+            <v>70</v>
+          </cell>
+          <cell r="AV124" t="str">
+            <v>A</v>
+          </cell>
+          <cell r="AW124" t="str">
+            <v>8</v>
+          </cell>
+          <cell r="AX124">
+            <v>4</v>
+          </cell>
+          <cell r="AY124">
+            <v>32</v>
+          </cell>
+          <cell r="AZ124">
+            <v>30</v>
+          </cell>
+          <cell r="BA124">
+            <v>40</v>
+          </cell>
+          <cell r="BB124">
+            <v>70</v>
+          </cell>
+          <cell r="BC124" t="str">
+            <v>A</v>
+          </cell>
+          <cell r="BD124" t="str">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="125">
+          <cell r="A125" t="str">
+            <v>MMS18-20/123</v>
+          </cell>
+          <cell r="B125" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+          <cell r="C125">
+            <v>0</v>
+          </cell>
+          <cell r="D125">
+            <v>0</v>
+          </cell>
+          <cell r="E125">
+            <v>0</v>
+          </cell>
+          <cell r="F125" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="G125" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="H125">
+            <v>4</v>
+          </cell>
+          <cell r="I125">
+            <v>0</v>
+          </cell>
+          <cell r="J125">
+            <v>0</v>
+          </cell>
+          <cell r="K125">
+            <v>0</v>
+          </cell>
+          <cell r="L125">
+            <v>0</v>
+          </cell>
+          <cell r="M125" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="N125" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="O125">
+            <v>4</v>
+          </cell>
+          <cell r="P125">
+            <v>0</v>
+          </cell>
+          <cell r="Q125">
+            <v>0</v>
+          </cell>
+          <cell r="R125">
+            <v>0</v>
+          </cell>
+          <cell r="S125">
+            <v>0</v>
+          </cell>
+          <cell r="T125" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="U125" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="V125">
+            <v>4</v>
+          </cell>
+          <cell r="W125">
+            <v>0</v>
+          </cell>
+          <cell r="X125">
+            <v>25</v>
+          </cell>
+          <cell r="Y125">
+            <v>35</v>
+          </cell>
+          <cell r="Z125">
+            <v>60</v>
+          </cell>
+          <cell r="AA125" t="str">
+            <v>B</v>
+          </cell>
+          <cell r="AB125" t="str">
+            <v>6</v>
+          </cell>
+          <cell r="AC125">
+            <v>4</v>
+          </cell>
+          <cell r="AD125">
+            <v>24</v>
+          </cell>
+          <cell r="AE125">
+            <v>25</v>
+          </cell>
+          <cell r="AF125">
+            <v>35</v>
+          </cell>
+          <cell r="AG125">
+            <v>60</v>
+          </cell>
+          <cell r="AH125" t="str">
+            <v>B</v>
+          </cell>
+          <cell r="AI125" t="str">
+            <v>6</v>
+          </cell>
+          <cell r="AJ125">
+            <v>4</v>
+          </cell>
+          <cell r="AK125">
+            <v>24</v>
+          </cell>
+          <cell r="AL125">
+            <v>25</v>
+          </cell>
+          <cell r="AM125">
+            <v>35</v>
+          </cell>
+          <cell r="AN125">
+            <v>60</v>
+          </cell>
+          <cell r="AO125" t="str">
+            <v>B</v>
+          </cell>
+          <cell r="AP125" t="str">
+            <v>6</v>
+          </cell>
+          <cell r="AQ125">
+            <v>4</v>
+          </cell>
+          <cell r="AR125">
+            <v>24</v>
+          </cell>
+          <cell r="AS125">
+            <v>25</v>
+          </cell>
+          <cell r="AT125">
+            <v>35</v>
+          </cell>
+          <cell r="AU125">
+            <v>60</v>
+          </cell>
+          <cell r="AV125" t="str">
+            <v>B</v>
+          </cell>
+          <cell r="AW125" t="str">
+            <v>6</v>
+          </cell>
+          <cell r="AX125">
+            <v>4</v>
+          </cell>
+          <cell r="AY125">
+            <v>24</v>
+          </cell>
+          <cell r="AZ125">
+            <v>25</v>
+          </cell>
+          <cell r="BA125">
+            <v>35</v>
+          </cell>
+          <cell r="BB125">
+            <v>60</v>
+          </cell>
+          <cell r="BC125" t="str">
+            <v>B</v>
+          </cell>
+          <cell r="BD125" t="str">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="126">
+          <cell r="A126" t="str">
+            <v>MMS18-20/124</v>
+          </cell>
+          <cell r="B126" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+          <cell r="C126">
+            <v>0</v>
+          </cell>
+          <cell r="D126">
+            <v>0</v>
+          </cell>
+          <cell r="E126">
+            <v>0</v>
+          </cell>
+          <cell r="F126" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="G126" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="H126">
+            <v>4</v>
+          </cell>
+          <cell r="I126">
+            <v>0</v>
+          </cell>
+          <cell r="J126">
+            <v>0</v>
+          </cell>
+          <cell r="K126">
+            <v>0</v>
+          </cell>
+          <cell r="L126">
+            <v>0</v>
+          </cell>
+          <cell r="M126" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="N126" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="O126">
+            <v>4</v>
+          </cell>
+          <cell r="P126">
+            <v>0</v>
+          </cell>
+          <cell r="Q126">
+            <v>0</v>
+          </cell>
+          <cell r="R126">
+            <v>0</v>
+          </cell>
+          <cell r="S126">
+            <v>0</v>
+          </cell>
+          <cell r="T126" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="U126" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="V126">
+            <v>4</v>
+          </cell>
+          <cell r="W126">
+            <v>0</v>
+          </cell>
+          <cell r="X126">
+            <v>32</v>
+          </cell>
+          <cell r="Y126">
+            <v>42</v>
+          </cell>
+          <cell r="Z126">
+            <v>74</v>
+          </cell>
+          <cell r="AA126" t="str">
+            <v>A</v>
+          </cell>
+          <cell r="AB126" t="str">
+            <v>8</v>
+          </cell>
+          <cell r="AC126">
+            <v>4</v>
+          </cell>
+          <cell r="AD126">
+            <v>32</v>
+          </cell>
+          <cell r="AE126">
+            <v>32</v>
+          </cell>
+          <cell r="AF126">
+            <v>42</v>
+          </cell>
+          <cell r="AG126">
+            <v>74</v>
+          </cell>
+          <cell r="AH126" t="str">
+            <v>A</v>
+          </cell>
+          <cell r="AI126" t="str">
+            <v>8</v>
+          </cell>
+          <cell r="AJ126">
+            <v>4</v>
+          </cell>
+          <cell r="AK126">
+            <v>32</v>
+          </cell>
+          <cell r="AL126">
+            <v>32</v>
+          </cell>
+          <cell r="AM126">
+            <v>42</v>
+          </cell>
+          <cell r="AN126">
+            <v>74</v>
+          </cell>
+          <cell r="AO126" t="str">
+            <v>A</v>
+          </cell>
+          <cell r="AP126" t="str">
+            <v>8</v>
+          </cell>
+          <cell r="AQ126">
+            <v>4</v>
+          </cell>
+          <cell r="AR126">
+            <v>32</v>
+          </cell>
+          <cell r="AS126">
+            <v>32</v>
+          </cell>
+          <cell r="AT126">
+            <v>42</v>
+          </cell>
+          <cell r="AU126">
+            <v>74</v>
+          </cell>
+          <cell r="AV126" t="str">
+            <v>A</v>
+          </cell>
+          <cell r="AW126" t="str">
+            <v>8</v>
+          </cell>
+          <cell r="AX126">
+            <v>4</v>
+          </cell>
+          <cell r="AY126">
+            <v>32</v>
+          </cell>
+          <cell r="AZ126">
+            <v>32</v>
+          </cell>
+          <cell r="BA126">
+            <v>42</v>
+          </cell>
+          <cell r="BB126">
+            <v>74</v>
+          </cell>
+          <cell r="BC126" t="str">
+            <v>A</v>
+          </cell>
+          <cell r="BD126" t="str">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="127">
+          <cell r="A127" t="str">
+            <v>MMS18-20/125</v>
+          </cell>
+          <cell r="B127" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+          <cell r="C127">
+            <v>0</v>
+          </cell>
+          <cell r="D127">
+            <v>0</v>
+          </cell>
+          <cell r="E127">
+            <v>0</v>
+          </cell>
+          <cell r="F127" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="G127" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="H127">
+            <v>4</v>
+          </cell>
+          <cell r="I127">
+            <v>0</v>
+          </cell>
+          <cell r="J127">
+            <v>0</v>
+          </cell>
+          <cell r="K127">
+            <v>0</v>
+          </cell>
+          <cell r="L127">
+            <v>0</v>
+          </cell>
+          <cell r="M127" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="N127" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="O127">
+            <v>4</v>
+          </cell>
+          <cell r="P127">
+            <v>0</v>
+          </cell>
+          <cell r="Q127">
+            <v>0</v>
+          </cell>
+          <cell r="R127">
+            <v>0</v>
+          </cell>
+          <cell r="S127">
+            <v>0</v>
+          </cell>
+          <cell r="T127" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="U127" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="V127">
+            <v>4</v>
+          </cell>
+          <cell r="W127">
+            <v>0</v>
+          </cell>
+          <cell r="X127">
+            <v>31</v>
+          </cell>
+          <cell r="Y127">
+            <v>45</v>
+          </cell>
+          <cell r="Z127">
+            <v>76</v>
+          </cell>
+          <cell r="AA127" t="str">
+            <v>A+</v>
+          </cell>
+          <cell r="AB127" t="str">
+            <v>9</v>
+          </cell>
+          <cell r="AC127">
+            <v>4</v>
+          </cell>
+          <cell r="AD127">
+            <v>36</v>
+          </cell>
+          <cell r="AE127">
+            <v>31</v>
+          </cell>
+          <cell r="AF127">
+            <v>45</v>
+          </cell>
+          <cell r="AG127">
+            <v>76</v>
+          </cell>
+          <cell r="AH127" t="str">
+            <v>A+</v>
+          </cell>
+          <cell r="AI127" t="str">
+            <v>9</v>
+          </cell>
+          <cell r="AJ127">
+            <v>4</v>
+          </cell>
+          <cell r="AK127">
+            <v>36</v>
+          </cell>
+          <cell r="AL127">
+            <v>31</v>
+          </cell>
+          <cell r="AM127">
+            <v>45</v>
+          </cell>
+          <cell r="AN127">
+            <v>76</v>
+          </cell>
+          <cell r="AO127" t="str">
+            <v>A+</v>
+          </cell>
+          <cell r="AP127" t="str">
+            <v>9</v>
+          </cell>
+          <cell r="AQ127">
+            <v>4</v>
+          </cell>
+          <cell r="AR127">
+            <v>36</v>
+          </cell>
+          <cell r="AS127">
+            <v>31</v>
+          </cell>
+          <cell r="AT127">
+            <v>45</v>
+          </cell>
+          <cell r="AU127">
+            <v>76</v>
+          </cell>
+          <cell r="AV127" t="str">
+            <v>A+</v>
+          </cell>
+          <cell r="AW127" t="str">
+            <v>9</v>
+          </cell>
+          <cell r="AX127">
+            <v>4</v>
+          </cell>
+          <cell r="AY127">
+            <v>36</v>
+          </cell>
+          <cell r="AZ127">
+            <v>31</v>
+          </cell>
+          <cell r="BA127">
+            <v>45</v>
+          </cell>
+          <cell r="BB127">
+            <v>76</v>
+          </cell>
+          <cell r="BC127" t="str">
+            <v>A+</v>
+          </cell>
+          <cell r="BD127" t="str">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="128">
+          <cell r="A128" t="str">
+            <v>MMS18-20/126</v>
+          </cell>
+          <cell r="B128" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+          <cell r="C128">
+            <v>0</v>
+          </cell>
+          <cell r="D128">
+            <v>0</v>
+          </cell>
+          <cell r="E128">
+            <v>0</v>
+          </cell>
+          <cell r="F128" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="G128" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="H128">
+            <v>4</v>
+          </cell>
+          <cell r="I128">
+            <v>0</v>
+          </cell>
+          <cell r="J128">
+            <v>0</v>
+          </cell>
+          <cell r="K128">
+            <v>0</v>
+          </cell>
+          <cell r="L128">
+            <v>0</v>
+          </cell>
+          <cell r="M128" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="N128" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="O128">
+            <v>4</v>
+          </cell>
+          <cell r="P128">
+            <v>0</v>
+          </cell>
+          <cell r="Q128">
+            <v>0</v>
+          </cell>
+          <cell r="R128">
+            <v>0</v>
+          </cell>
+          <cell r="S128">
+            <v>0</v>
+          </cell>
+          <cell r="T128" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="U128" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="V128">
+            <v>4</v>
+          </cell>
+          <cell r="W128">
+            <v>0</v>
+          </cell>
+          <cell r="X128">
+            <v>33</v>
+          </cell>
+          <cell r="Y128">
+            <v>36</v>
+          </cell>
+          <cell r="Z128">
+            <v>69</v>
+          </cell>
+          <cell r="AA128" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="AB128" t="str">
+            <v>7</v>
+          </cell>
+          <cell r="AC128">
+            <v>4</v>
+          </cell>
+          <cell r="AD128">
+            <v>28</v>
+          </cell>
+          <cell r="AE128">
+            <v>33</v>
+          </cell>
+          <cell r="AF128">
+            <v>36</v>
+          </cell>
+          <cell r="AG128">
+            <v>69</v>
+          </cell>
+          <cell r="AH128" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="AI128" t="str">
+            <v>7</v>
+          </cell>
+          <cell r="AJ128">
+            <v>4</v>
+          </cell>
+          <cell r="AK128">
+            <v>28</v>
+          </cell>
+          <cell r="AL128">
+            <v>33</v>
+          </cell>
+          <cell r="AM128">
+            <v>36</v>
+          </cell>
+          <cell r="AN128">
+            <v>69</v>
+          </cell>
+          <cell r="AO128" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="AP128" t="str">
+            <v>7</v>
+          </cell>
+          <cell r="AQ128">
+            <v>4</v>
+          </cell>
+          <cell r="AR128">
+            <v>28</v>
+          </cell>
+          <cell r="AS128">
+            <v>33</v>
+          </cell>
+          <cell r="AT128">
+            <v>36</v>
+          </cell>
+          <cell r="AU128">
+            <v>69</v>
+          </cell>
+          <cell r="AV128" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="AW128" t="str">
+            <v>7</v>
+          </cell>
+          <cell r="AX128">
+            <v>4</v>
+          </cell>
+          <cell r="AY128">
+            <v>28</v>
+          </cell>
+          <cell r="AZ128">
+            <v>33</v>
+          </cell>
+          <cell r="BA128">
+            <v>36</v>
+          </cell>
+          <cell r="BB128">
+            <v>69</v>
+          </cell>
+          <cell r="BC128" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="BD128" t="str">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="129">
+          <cell r="A129" t="str">
+            <v>MMS18-20/127</v>
+          </cell>
+          <cell r="B129" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+          <cell r="C129">
+            <v>0</v>
+          </cell>
+          <cell r="D129">
+            <v>0</v>
+          </cell>
+          <cell r="E129">
+            <v>0</v>
+          </cell>
+          <cell r="F129" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="G129" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="H129">
+            <v>4</v>
+          </cell>
+          <cell r="I129">
+            <v>0</v>
+          </cell>
+          <cell r="J129">
+            <v>0</v>
+          </cell>
+          <cell r="K129">
+            <v>0</v>
+          </cell>
+          <cell r="L129">
+            <v>0</v>
+          </cell>
+          <cell r="M129" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="N129" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="O129">
+            <v>4</v>
+          </cell>
+          <cell r="P129">
+            <v>0</v>
+          </cell>
+          <cell r="Q129">
+            <v>0</v>
+          </cell>
+          <cell r="R129">
+            <v>0</v>
+          </cell>
+          <cell r="S129">
+            <v>0</v>
+          </cell>
+          <cell r="T129" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="U129" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="V129">
+            <v>4</v>
+          </cell>
+          <cell r="W129">
+            <v>0</v>
+          </cell>
+          <cell r="X129">
+            <v>32</v>
+          </cell>
+          <cell r="Y129">
+            <v>39</v>
+          </cell>
+          <cell r="Z129">
+            <v>71</v>
+          </cell>
+          <cell r="AA129" t="str">
+            <v>A</v>
+          </cell>
+          <cell r="AB129" t="str">
+            <v>8</v>
+          </cell>
+          <cell r="AC129">
+            <v>4</v>
+          </cell>
+          <cell r="AD129">
+            <v>32</v>
+          </cell>
+          <cell r="AE129">
+            <v>32</v>
+          </cell>
+          <cell r="AF129">
+            <v>39</v>
+          </cell>
+          <cell r="AG129">
+            <v>71</v>
+          </cell>
+          <cell r="AH129" t="str">
+            <v>A</v>
+          </cell>
+          <cell r="AI129" t="str">
+            <v>8</v>
+          </cell>
+          <cell r="AJ129">
+            <v>4</v>
+          </cell>
+          <cell r="AK129">
+            <v>32</v>
+          </cell>
+          <cell r="AL129">
+            <v>32</v>
+          </cell>
+          <cell r="AM129">
+            <v>39</v>
+          </cell>
+          <cell r="AN129">
+            <v>71</v>
+          </cell>
+          <cell r="AO129" t="str">
+            <v>A</v>
+          </cell>
+          <cell r="AP129" t="str">
+            <v>8</v>
+          </cell>
+          <cell r="AQ129">
+            <v>4</v>
+          </cell>
+          <cell r="AR129">
+            <v>32</v>
+          </cell>
+          <cell r="AS129">
+            <v>32</v>
+          </cell>
+          <cell r="AT129">
+            <v>39</v>
+          </cell>
+          <cell r="AU129">
+            <v>71</v>
+          </cell>
+          <cell r="AV129" t="str">
+            <v>A</v>
+          </cell>
+          <cell r="AW129" t="str">
+            <v>8</v>
+          </cell>
+          <cell r="AX129">
+            <v>4</v>
+          </cell>
+          <cell r="AY129">
+            <v>32</v>
+          </cell>
+          <cell r="AZ129">
+            <v>32</v>
+          </cell>
+          <cell r="BA129">
+            <v>39</v>
+          </cell>
+          <cell r="BB129">
+            <v>71</v>
+          </cell>
+          <cell r="BC129" t="str">
+            <v>A</v>
+          </cell>
+          <cell r="BD129" t="str">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="130">
+          <cell r="A130" t="str">
+            <v>MMS18-20/128</v>
+          </cell>
+          <cell r="B130" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+          <cell r="C130">
+            <v>0</v>
+          </cell>
+          <cell r="D130">
+            <v>0</v>
+          </cell>
+          <cell r="E130">
+            <v>0</v>
+          </cell>
+          <cell r="F130" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="G130" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="H130">
+            <v>4</v>
+          </cell>
+          <cell r="I130">
+            <v>0</v>
+          </cell>
+          <cell r="J130">
+            <v>0</v>
+          </cell>
+          <cell r="K130">
+            <v>0</v>
+          </cell>
+          <cell r="L130">
+            <v>0</v>
+          </cell>
+          <cell r="M130" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="N130" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="O130">
+            <v>4</v>
+          </cell>
+          <cell r="P130">
+            <v>0</v>
+          </cell>
+          <cell r="Q130">
+            <v>0</v>
+          </cell>
+          <cell r="R130">
+            <v>0</v>
+          </cell>
+          <cell r="S130">
+            <v>0</v>
+          </cell>
+          <cell r="T130" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="U130" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="V130">
+            <v>4</v>
+          </cell>
+          <cell r="W130">
+            <v>0</v>
+          </cell>
+          <cell r="X130">
+            <v>30</v>
+          </cell>
+          <cell r="Y130">
+            <v>41</v>
+          </cell>
+          <cell r="Z130">
+            <v>71</v>
+          </cell>
+          <cell r="AA130" t="str">
+            <v>A</v>
+          </cell>
+          <cell r="AB130" t="str">
+            <v>8</v>
+          </cell>
+          <cell r="AC130">
+            <v>4</v>
+          </cell>
+          <cell r="AD130">
+            <v>32</v>
+          </cell>
+          <cell r="AE130">
+            <v>30</v>
+          </cell>
+          <cell r="AF130">
+            <v>41</v>
+          </cell>
+          <cell r="AG130">
+            <v>71</v>
+          </cell>
+          <cell r="AH130" t="str">
+            <v>A</v>
+          </cell>
+          <cell r="AI130" t="str">
+            <v>8</v>
+          </cell>
+          <cell r="AJ130">
+            <v>4</v>
+          </cell>
+          <cell r="AK130">
+            <v>32</v>
+          </cell>
+          <cell r="AL130">
+            <v>30</v>
+          </cell>
+          <cell r="AM130">
+            <v>41</v>
+          </cell>
+          <cell r="AN130">
+            <v>71</v>
+          </cell>
+          <cell r="AO130" t="str">
+            <v>A</v>
+          </cell>
+          <cell r="AP130" t="str">
+            <v>8</v>
+          </cell>
+          <cell r="AQ130">
+            <v>4</v>
+          </cell>
+          <cell r="AR130">
+            <v>32</v>
+          </cell>
+          <cell r="AS130">
+            <v>30</v>
+          </cell>
+          <cell r="AT130">
+            <v>41</v>
+          </cell>
+          <cell r="AU130">
+            <v>71</v>
+          </cell>
+          <cell r="AV130" t="str">
+            <v>A</v>
+          </cell>
+          <cell r="AW130" t="str">
+            <v>8</v>
+          </cell>
+          <cell r="AX130">
+            <v>4</v>
+          </cell>
+          <cell r="AY130">
+            <v>32</v>
+          </cell>
+          <cell r="AZ130">
+            <v>30</v>
+          </cell>
+          <cell r="BA130">
+            <v>41</v>
+          </cell>
+          <cell r="BB130">
+            <v>71</v>
+          </cell>
+          <cell r="BC130" t="str">
+            <v>A</v>
+          </cell>
+          <cell r="BD130" t="str">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="131">
+          <cell r="A131" t="str">
+            <v>MMS18-20/129</v>
+          </cell>
+          <cell r="B131" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+          <cell r="C131">
+            <v>0</v>
+          </cell>
+          <cell r="D131">
+            <v>0</v>
+          </cell>
+          <cell r="E131">
+            <v>0</v>
+          </cell>
+          <cell r="F131" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="G131" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="H131">
+            <v>4</v>
+          </cell>
+          <cell r="I131">
+            <v>0</v>
+          </cell>
+          <cell r="J131">
+            <v>0</v>
+          </cell>
+          <cell r="K131">
+            <v>0</v>
+          </cell>
+          <cell r="L131">
+            <v>0</v>
+          </cell>
+          <cell r="M131" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="N131" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="O131">
+            <v>4</v>
+          </cell>
+          <cell r="P131">
+            <v>0</v>
+          </cell>
+          <cell r="Q131">
+            <v>0</v>
+          </cell>
+          <cell r="R131">
+            <v>0</v>
+          </cell>
+          <cell r="S131">
+            <v>0</v>
+          </cell>
+          <cell r="T131" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="U131" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="V131">
+            <v>4</v>
+          </cell>
+          <cell r="W131">
+            <v>0</v>
+          </cell>
+          <cell r="X131">
+            <v>29</v>
+          </cell>
+          <cell r="Y131">
+            <v>46</v>
+          </cell>
+          <cell r="Z131">
+            <v>75</v>
+          </cell>
+          <cell r="AA131" t="str">
+            <v>A+</v>
+          </cell>
+          <cell r="AB131" t="str">
+            <v>9</v>
+          </cell>
+          <cell r="AC131">
+            <v>4</v>
+          </cell>
+          <cell r="AD131">
+            <v>36</v>
+          </cell>
+          <cell r="AE131">
+            <v>29</v>
+          </cell>
+          <cell r="AF131">
+            <v>46</v>
+          </cell>
+          <cell r="AG131">
+            <v>75</v>
+          </cell>
+          <cell r="AH131" t="str">
+            <v>A+</v>
+          </cell>
+          <cell r="AI131" t="str">
+            <v>9</v>
+          </cell>
+          <cell r="AJ131">
+            <v>4</v>
+          </cell>
+          <cell r="AK131">
+            <v>36</v>
+          </cell>
+          <cell r="AL131">
+            <v>29</v>
+          </cell>
+          <cell r="AM131">
+            <v>46</v>
+          </cell>
+          <cell r="AN131">
+            <v>75</v>
+          </cell>
+          <cell r="AO131" t="str">
+            <v>A+</v>
+          </cell>
+          <cell r="AP131" t="str">
+            <v>9</v>
+          </cell>
+          <cell r="AQ131">
+            <v>4</v>
+          </cell>
+          <cell r="AR131">
+            <v>36</v>
+          </cell>
+          <cell r="AS131">
+            <v>29</v>
+          </cell>
+          <cell r="AT131">
+            <v>46</v>
+          </cell>
+          <cell r="AU131">
+            <v>75</v>
+          </cell>
+          <cell r="AV131" t="str">
+            <v>A+</v>
+          </cell>
+          <cell r="AW131" t="str">
+            <v>9</v>
+          </cell>
+          <cell r="AX131">
+            <v>4</v>
+          </cell>
+          <cell r="AY131">
+            <v>36</v>
+          </cell>
+          <cell r="AZ131">
+            <v>29</v>
+          </cell>
+          <cell r="BA131">
+            <v>46</v>
+          </cell>
+          <cell r="BB131">
+            <v>75</v>
+          </cell>
+          <cell r="BC131" t="str">
+            <v>A+</v>
+          </cell>
+          <cell r="BD131" t="str">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="132">
+          <cell r="A132" t="str">
+            <v>MMS18-20/130</v>
+          </cell>
+          <cell r="B132" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+          <cell r="C132">
+            <v>0</v>
+          </cell>
+          <cell r="D132">
+            <v>0</v>
+          </cell>
+          <cell r="E132">
+            <v>0</v>
+          </cell>
+          <cell r="F132" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="G132" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="H132">
+            <v>4</v>
+          </cell>
+          <cell r="I132">
+            <v>0</v>
+          </cell>
+          <cell r="J132">
+            <v>0</v>
+          </cell>
+          <cell r="K132">
+            <v>0</v>
+          </cell>
+          <cell r="L132">
+            <v>0</v>
+          </cell>
+          <cell r="M132" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="N132" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="O132">
+            <v>4</v>
+          </cell>
+          <cell r="P132">
+            <v>0</v>
+          </cell>
+          <cell r="Q132">
+            <v>0</v>
+          </cell>
+          <cell r="R132">
+            <v>0</v>
+          </cell>
+          <cell r="S132">
+            <v>0</v>
+          </cell>
+          <cell r="T132" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="U132" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="V132">
+            <v>4</v>
+          </cell>
+          <cell r="W132">
+            <v>0</v>
+          </cell>
+          <cell r="X132">
+            <v>27</v>
+          </cell>
+          <cell r="Y132">
+            <v>40</v>
+          </cell>
+          <cell r="Z132">
+            <v>67</v>
+          </cell>
+          <cell r="AA132" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="AB132" t="str">
+            <v>7</v>
+          </cell>
+          <cell r="AC132">
+            <v>4</v>
+          </cell>
+          <cell r="AD132">
+            <v>28</v>
+          </cell>
+          <cell r="AE132">
+            <v>27</v>
+          </cell>
+          <cell r="AF132">
+            <v>40</v>
+          </cell>
+          <cell r="AG132">
+            <v>67</v>
+          </cell>
+          <cell r="AH132" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="AI132" t="str">
+            <v>7</v>
+          </cell>
+          <cell r="AJ132">
+            <v>4</v>
+          </cell>
+          <cell r="AK132">
+            <v>28</v>
+          </cell>
+          <cell r="AL132">
+            <v>27</v>
+          </cell>
+          <cell r="AM132">
+            <v>40</v>
+          </cell>
+          <cell r="AN132">
+            <v>67</v>
+          </cell>
+          <cell r="AO132" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="AP132" t="str">
+            <v>7</v>
+          </cell>
+          <cell r="AQ132">
+            <v>4</v>
+          </cell>
+          <cell r="AR132">
+            <v>28</v>
+          </cell>
+          <cell r="AS132">
+            <v>27</v>
+          </cell>
+          <cell r="AT132">
+            <v>40</v>
+          </cell>
+          <cell r="AU132">
+            <v>67</v>
+          </cell>
+          <cell r="AV132" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="AW132" t="str">
+            <v>7</v>
+          </cell>
+          <cell r="AX132">
+            <v>4</v>
+          </cell>
+          <cell r="AY132">
+            <v>28</v>
+          </cell>
+          <cell r="AZ132">
+            <v>27</v>
+          </cell>
+          <cell r="BA132">
+            <v>40</v>
+          </cell>
+          <cell r="BB132">
+            <v>67</v>
+          </cell>
+          <cell r="BC132" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="BD132" t="str">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="133">
+          <cell r="A133" t="str">
+            <v>MMS18-20/131</v>
+          </cell>
+          <cell r="B133" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+          <cell r="C133">
+            <v>0</v>
+          </cell>
+          <cell r="D133">
+            <v>0</v>
+          </cell>
+          <cell r="E133">
+            <v>0</v>
+          </cell>
+          <cell r="F133" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="G133" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="H133">
+            <v>4</v>
+          </cell>
+          <cell r="I133">
+            <v>0</v>
+          </cell>
+          <cell r="J133">
+            <v>0</v>
+          </cell>
+          <cell r="K133">
+            <v>0</v>
+          </cell>
+          <cell r="L133">
+            <v>0</v>
+          </cell>
+          <cell r="M133" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="N133" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="O133">
+            <v>4</v>
+          </cell>
+          <cell r="P133">
+            <v>0</v>
+          </cell>
+          <cell r="Q133">
+            <v>0</v>
+          </cell>
+          <cell r="R133">
+            <v>0</v>
+          </cell>
+          <cell r="S133">
+            <v>0</v>
+          </cell>
+          <cell r="T133" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="U133" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="V133">
+            <v>4</v>
+          </cell>
+          <cell r="W133">
+            <v>0</v>
+          </cell>
+          <cell r="X133">
+            <v>31</v>
+          </cell>
+          <cell r="Y133">
+            <v>38</v>
+          </cell>
+          <cell r="Z133">
+            <v>69</v>
+          </cell>
+          <cell r="AA133" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="AB133" t="str">
+            <v>7</v>
+          </cell>
+          <cell r="AC133">
+            <v>4</v>
+          </cell>
+          <cell r="AD133">
+            <v>28</v>
+          </cell>
+          <cell r="AE133">
+            <v>31</v>
+          </cell>
+          <cell r="AF133">
+            <v>38</v>
+          </cell>
+          <cell r="AG133">
+            <v>69</v>
+          </cell>
+          <cell r="AH133" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="AI133" t="str">
+            <v>7</v>
+          </cell>
+          <cell r="AJ133">
+            <v>4</v>
+          </cell>
+          <cell r="AK133">
+            <v>28</v>
+          </cell>
+          <cell r="AL133">
+            <v>31</v>
+          </cell>
+          <cell r="AM133">
+            <v>38</v>
+          </cell>
+          <cell r="AN133">
+            <v>69</v>
+          </cell>
+          <cell r="AO133" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="AP133" t="str">
+            <v>7</v>
+          </cell>
+          <cell r="AQ133">
+            <v>4</v>
+          </cell>
+          <cell r="AR133">
+            <v>28</v>
+          </cell>
+          <cell r="AS133">
+            <v>31</v>
+          </cell>
+          <cell r="AT133">
+            <v>38</v>
+          </cell>
+          <cell r="AU133">
+            <v>69</v>
+          </cell>
+          <cell r="AV133" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="AW133" t="str">
+            <v>7</v>
+          </cell>
+          <cell r="AX133">
+            <v>4</v>
+          </cell>
+          <cell r="AY133">
+            <v>28</v>
+          </cell>
+          <cell r="AZ133">
+            <v>31</v>
+          </cell>
+          <cell r="BA133">
+            <v>38</v>
+          </cell>
+          <cell r="BB133">
+            <v>69</v>
+          </cell>
+          <cell r="BC133" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="BD133" t="str">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="134">
+          <cell r="A134" t="str">
+            <v>MMS18-20/132</v>
+          </cell>
+          <cell r="B134" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+          <cell r="C134">
+            <v>0</v>
+          </cell>
+          <cell r="D134">
+            <v>0</v>
+          </cell>
+          <cell r="E134">
+            <v>0</v>
+          </cell>
+          <cell r="F134" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="G134" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="H134">
+            <v>4</v>
+          </cell>
+          <cell r="I134">
+            <v>0</v>
+          </cell>
+          <cell r="J134">
+            <v>0</v>
+          </cell>
+          <cell r="K134">
+            <v>0</v>
+          </cell>
+          <cell r="L134">
+            <v>0</v>
+          </cell>
+          <cell r="M134" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="N134" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="O134">
+            <v>4</v>
+          </cell>
+          <cell r="P134">
+            <v>0</v>
+          </cell>
+          <cell r="Q134">
+            <v>0</v>
+          </cell>
+          <cell r="R134">
+            <v>0</v>
+          </cell>
+          <cell r="S134">
+            <v>0</v>
+          </cell>
+          <cell r="T134" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="U134" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="V134">
+            <v>4</v>
+          </cell>
+          <cell r="W134">
+            <v>0</v>
+          </cell>
+          <cell r="X134">
+            <v>28</v>
+          </cell>
+          <cell r="Y134">
+            <v>37</v>
+          </cell>
+          <cell r="Z134">
+            <v>65</v>
+          </cell>
+          <cell r="AA134" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="AB134" t="str">
+            <v>7</v>
+          </cell>
+          <cell r="AC134">
+            <v>4</v>
+          </cell>
+          <cell r="AD134">
+            <v>28</v>
+          </cell>
+          <cell r="AE134">
+            <v>28</v>
+          </cell>
+          <cell r="AF134">
+            <v>37</v>
+          </cell>
+          <cell r="AG134">
+            <v>65</v>
+          </cell>
+          <cell r="AH134" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="AI134" t="str">
+            <v>7</v>
+          </cell>
+          <cell r="AJ134">
+            <v>4</v>
+          </cell>
+          <cell r="AK134">
+            <v>28</v>
+          </cell>
+          <cell r="AL134">
+            <v>28</v>
+          </cell>
+          <cell r="AM134">
+            <v>37</v>
+          </cell>
+          <cell r="AN134">
+            <v>65</v>
+          </cell>
+          <cell r="AO134" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="AP134" t="str">
+            <v>7</v>
+          </cell>
+          <cell r="AQ134">
+            <v>4</v>
+          </cell>
+          <cell r="AR134">
+            <v>28</v>
+          </cell>
+          <cell r="AS134">
+            <v>28</v>
+          </cell>
+          <cell r="AT134">
+            <v>37</v>
+          </cell>
+          <cell r="AU134">
+            <v>65</v>
+          </cell>
+          <cell r="AV134" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="AW134" t="str">
+            <v>7</v>
+          </cell>
+          <cell r="AX134">
+            <v>4</v>
+          </cell>
+          <cell r="AY134">
+            <v>28</v>
+          </cell>
+          <cell r="AZ134">
+            <v>28</v>
+          </cell>
+          <cell r="BA134">
+            <v>37</v>
+          </cell>
+          <cell r="BB134">
+            <v>65</v>
+          </cell>
+          <cell r="BC134" t="str">
+            <v>B+</v>
+          </cell>
+          <cell r="BD134" t="str">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="135">
+          <cell r="A135" t="str">
+            <v>MMS18-20/133</v>
+          </cell>
+          <cell r="B135" t="str">
+            <v>*** (NOT AVAILABLE) ***</v>
+          </cell>
+          <cell r="C135">
+            <v>0</v>
+          </cell>
+          <cell r="D135">
+            <v>0</v>
+          </cell>
+          <cell r="E135">
+            <v>0</v>
+          </cell>
+          <cell r="F135" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="G135" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="H135">
+            <v>4</v>
+          </cell>
+          <cell r="I135">
+            <v>0</v>
+          </cell>
+          <cell r="J135">
+            <v>0</v>
+          </cell>
+          <cell r="K135">
+            <v>0</v>
+          </cell>
+          <cell r="L135">
+            <v>0</v>
+          </cell>
+          <cell r="M135" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="N135" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="O135">
+            <v>4</v>
+          </cell>
+          <cell r="P135">
+            <v>0</v>
+          </cell>
+          <cell r="Q135">
+            <v>0</v>
+          </cell>
+          <cell r="R135">
+            <v>0</v>
+          </cell>
+          <cell r="S135">
+            <v>0</v>
+          </cell>
+          <cell r="T135" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="U135" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="V135">
+            <v>4</v>
+          </cell>
+          <cell r="W135">
+            <v>0</v>
+          </cell>
+          <cell r="X135">
+            <v>0</v>
+          </cell>
+          <cell r="Y135">
+            <v>0</v>
+          </cell>
+          <cell r="Z135">
+            <v>0</v>
+          </cell>
+          <cell r="AA135" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="AB135" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="AC135">
+            <v>4</v>
+          </cell>
+          <cell r="AD135">
+            <v>0</v>
+          </cell>
+          <cell r="AE135">
+            <v>0</v>
+          </cell>
+          <cell r="AF135">
+            <v>0</v>
+          </cell>
+          <cell r="AG135">
+            <v>0</v>
+          </cell>
+          <cell r="AH135" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="AI135" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="AJ135">
+            <v>4</v>
+          </cell>
+          <cell r="AK135">
+            <v>0</v>
+          </cell>
+          <cell r="AL135">
+            <v>0</v>
+          </cell>
+          <cell r="AM135">
+            <v>0</v>
+          </cell>
+          <cell r="AN135">
+            <v>0</v>
+          </cell>
+          <cell r="AO135" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="AP135" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="AQ135">
+            <v>4</v>
+          </cell>
+          <cell r="AR135">
+            <v>0</v>
+          </cell>
+          <cell r="AS135">
+            <v>0</v>
+          </cell>
+          <cell r="AT135">
+            <v>0</v>
+          </cell>
+          <cell r="AU135">
+            <v>0</v>
+          </cell>
+          <cell r="AV135" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="AW135" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="AX135">
+            <v>4</v>
+          </cell>
+          <cell r="AY135">
+            <v>0</v>
+          </cell>
+          <cell r="AZ135">
+            <v>0</v>
+          </cell>
+          <cell r="BA135">
+            <v>0</v>
+          </cell>
+          <cell r="BB135">
+            <v>0</v>
+          </cell>
+          <cell r="BC135" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="BD135" t="str">
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
@@ -27127,7 +29441,7 @@
       <c r="C9" s="9"/>
       <c r="D9" s="8" t="str">
         <f>VLOOKUP(D13,[1]Sheet1!$A:$B,2,0)</f>
-        <v>CHAWHAN SAMTA VIJAY SUNITA</v>
+        <v>ADEPU CHETAN GANESH ARCHANA</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
@@ -27344,8 +29658,8 @@
         <v>20</v>
       </c>
       <c r="G17" s="3">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$C$122,3,0)</f>
-        <v>27</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$C$135,3,0)</f>
+        <v>40</v>
       </c>
       <c r="H17" s="3">
         <v>60</v>
@@ -27354,8 +29668,8 @@
         <v>30</v>
       </c>
       <c r="J17" s="3">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$D$122,4,0)</f>
-        <v>40</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$D$135,4,0)</f>
+        <v>60</v>
       </c>
       <c r="K17" s="3">
         <v>100</v>
@@ -27365,25 +29679,25 @@
       </c>
       <c r="M17" s="3">
         <f>SUM(G17,J17)</f>
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="N17" s="3">
         <v>4</v>
       </c>
       <c r="O17" s="3" t="str">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$F$122,6,0)</f>
-        <v>B+</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$F$135,6,0)</f>
+        <v>O</v>
       </c>
       <c r="P17" s="3">
         <v>4</v>
       </c>
       <c r="Q17" s="3" t="str">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$G$122,7,0)</f>
-        <v>7</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$G$135,7,0)</f>
+        <v>10</v>
       </c>
       <c r="R17" s="3">
         <f>P17*Q17</f>
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -27402,8 +29716,8 @@
         <v>20</v>
       </c>
       <c r="G18" s="3">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$J$122,10,0)</f>
-        <v>27</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$J$135,10,0)</f>
+        <v>40</v>
       </c>
       <c r="H18" s="3">
         <v>60</v>
@@ -27412,8 +29726,8 @@
         <v>30</v>
       </c>
       <c r="J18" s="3">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$K$122,11,0)</f>
-        <v>40</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$K$135,11,0)</f>
+        <v>60</v>
       </c>
       <c r="K18" s="3">
         <v>100</v>
@@ -27423,25 +29737,25 @@
       </c>
       <c r="M18" s="3">
         <f t="shared" ref="M18:M24" si="0">SUM(G18,J18)</f>
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="N18" s="3">
         <v>4</v>
       </c>
       <c r="O18" s="3" t="str">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$M$122,13,0)</f>
-        <v>B+</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$M$135,13,0)</f>
+        <v>O</v>
       </c>
       <c r="P18" s="3">
         <v>4</v>
       </c>
       <c r="Q18" s="3" t="str">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$N$122,14,0)</f>
-        <v>7</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$N$135,14,0)</f>
+        <v>10</v>
       </c>
       <c r="R18" s="3">
         <f t="shared" ref="R18:R24" si="1">P18*Q18</f>
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -27460,8 +29774,8 @@
         <v>20</v>
       </c>
       <c r="G19" s="3">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$Q$122,17,0)</f>
-        <v>27</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$Q$135,17,0)</f>
+        <v>30</v>
       </c>
       <c r="H19" s="3">
         <v>60</v>
@@ -27470,7 +29784,7 @@
         <v>30</v>
       </c>
       <c r="J19" s="3">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$R$122,18,0)</f>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$R$135,18,0)</f>
         <v>40</v>
       </c>
       <c r="K19" s="3">
@@ -27481,25 +29795,25 @@
       </c>
       <c r="M19" s="3">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N19" s="3">
         <v>4</v>
       </c>
       <c r="O19" s="3" t="str">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$T$122,20,0)</f>
-        <v>A</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$T$135,20,0)</f>
+        <v>A+</v>
       </c>
       <c r="P19" s="3">
         <v>4</v>
       </c>
       <c r="Q19" s="3" t="str">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$U$122,21,0)</f>
-        <v>7</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$U$135,21,0)</f>
+        <v>8</v>
       </c>
       <c r="R19" s="3">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -27518,8 +29832,8 @@
         <v>20</v>
       </c>
       <c r="G20" s="3">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$X$122,24,0)</f>
-        <v>27</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$X$135,24,0)</f>
+        <v>30</v>
       </c>
       <c r="H20" s="3">
         <v>60</v>
@@ -27528,7 +29842,7 @@
         <v>30</v>
       </c>
       <c r="J20" s="3">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$Y$122,25,0)</f>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$Y$135,25,0)</f>
         <v>40</v>
       </c>
       <c r="K20" s="3">
@@ -27539,25 +29853,25 @@
       </c>
       <c r="M20" s="3">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N20" s="3">
         <v>4</v>
       </c>
       <c r="O20" s="3" t="str">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AA$122,27,0)</f>
-        <v>B+</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AA$135,27,0)</f>
+        <v>A</v>
       </c>
       <c r="P20" s="3">
         <v>4</v>
       </c>
       <c r="Q20" s="3" t="str">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AB$122,28,0)</f>
-        <v>7</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AB$135,28,0)</f>
+        <v>8</v>
       </c>
       <c r="R20" s="3">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
@@ -27576,8 +29890,8 @@
         <v>20</v>
       </c>
       <c r="G21" s="3">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AE$122,31,0)</f>
-        <v>27</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AE$135,31,0)</f>
+        <v>30</v>
       </c>
       <c r="H21" s="3">
         <v>60</v>
@@ -27586,7 +29900,7 @@
         <v>30</v>
       </c>
       <c r="J21" s="3">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AF$122,32,0)</f>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AF$135,32,0)</f>
         <v>40</v>
       </c>
       <c r="K21" s="3">
@@ -27597,25 +29911,25 @@
       </c>
       <c r="M21" s="3">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N21" s="3">
         <v>4</v>
       </c>
       <c r="O21" s="3" t="str">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AH$122,34,0)</f>
-        <v>B+</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AH$135,34,0)</f>
+        <v>A</v>
       </c>
       <c r="P21" s="3">
         <v>4</v>
       </c>
       <c r="Q21" s="3" t="str">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AI$122,35,0)</f>
-        <v>7</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AI$135,35,0)</f>
+        <v>8</v>
       </c>
       <c r="R21" s="3">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -27634,8 +29948,8 @@
         <v>20</v>
       </c>
       <c r="G22" s="3">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AL$122,38,0)</f>
-        <v>27</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AL$135,38,0)</f>
+        <v>30</v>
       </c>
       <c r="H22" s="3">
         <v>60</v>
@@ -27644,7 +29958,7 @@
         <v>30</v>
       </c>
       <c r="J22" s="3">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AM$122,39,0)</f>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AM$135,39,0)</f>
         <v>40</v>
       </c>
       <c r="K22" s="3">
@@ -27655,25 +29969,25 @@
       </c>
       <c r="M22" s="3">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N22" s="3">
         <v>4</v>
       </c>
       <c r="O22" s="3" t="str">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AO$122,41,0)</f>
-        <v>B+</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AO$135,41,0)</f>
+        <v>A</v>
       </c>
       <c r="P22" s="3">
         <v>4</v>
       </c>
       <c r="Q22" s="3" t="str">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AP$122,42,0)</f>
-        <v>7</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AP$135,42,0)</f>
+        <v>8</v>
       </c>
       <c r="R22" s="3">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -27692,8 +30006,8 @@
         <v>20</v>
       </c>
       <c r="G23" s="3">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AS$122,45,0)</f>
-        <v>27</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AS$135,45,0)</f>
+        <v>30</v>
       </c>
       <c r="H23" s="3">
         <v>60</v>
@@ -27702,7 +30016,7 @@
         <v>30</v>
       </c>
       <c r="J23" s="3">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AT$122,46,0)</f>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AT$135,46,0)</f>
         <v>40</v>
       </c>
       <c r="K23" s="3">
@@ -27713,25 +30027,25 @@
       </c>
       <c r="M23" s="3">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N23" s="3">
         <v>4</v>
       </c>
       <c r="O23" s="3" t="str">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AV$122,48,0)</f>
-        <v>B+</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AV$135,48,0)</f>
+        <v>A</v>
       </c>
       <c r="P23" s="3">
         <v>4</v>
       </c>
       <c r="Q23" s="3" t="str">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AW$122,49,0)</f>
-        <v>7</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AW$135,49,0)</f>
+        <v>8</v>
       </c>
       <c r="R23" s="3">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -27750,8 +30064,8 @@
         <v>20</v>
       </c>
       <c r="G24" s="3">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AZ$122,52,0)</f>
-        <v>27</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$AZ$135,52,0)</f>
+        <v>30</v>
       </c>
       <c r="H24" s="3">
         <v>60</v>
@@ -27760,7 +30074,7 @@
         <v>30</v>
       </c>
       <c r="J24" s="3">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$BA$122,53,0)</f>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$BA$135,53,0)</f>
         <v>40</v>
       </c>
       <c r="K24" s="3">
@@ -27771,25 +30085,25 @@
       </c>
       <c r="M24" s="3">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N24" s="3">
         <v>4</v>
       </c>
       <c r="O24" s="3" t="str">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$BC$122,55,0)</f>
-        <v>B+</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$BC$135,55,0)</f>
+        <v>A</v>
       </c>
       <c r="P24" s="3">
         <v>4</v>
       </c>
       <c r="Q24" s="3" t="str">
-        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$BD$122,56,0)</f>
-        <v>7</v>
+        <f>VLOOKUP(D13,'[2]Subject Marks'!$A$3:$BD$135,56,0)</f>
+        <v>8</v>
       </c>
       <c r="R24" s="3">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -27811,7 +30125,7 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3">
         <f>SUM(M17:M24)</f>
-        <v>536</v>
+        <v>620</v>
       </c>
       <c r="N25" s="3"/>
       <c r="O25" s="7"/>
@@ -27821,7 +30135,7 @@
       <c r="Q25" s="7"/>
       <c r="R25" s="7">
         <f>SUM(R17:R24)</f>
-        <v>224</v>
+        <v>272</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -27843,17 +30157,17 @@
       <c r="M26" s="12"/>
       <c r="N26" s="12" t="str">
         <f>"SGPI : "&amp;VLOOKUP(D13,'[2]Subject Marks'!$A$3:$BN$122,66,0)</f>
-        <v>SGPI : 7</v>
+        <v>SGPI : 8.5</v>
       </c>
       <c r="O26" s="12"/>
       <c r="P26" s="13" t="str">
         <f>"Overall Grade:"&amp;VLOOKUP(D13,'[2]Subject Marks'!$A$3:$BO$122,67,0)</f>
-        <v>Overall Grade:B+</v>
+        <v>Overall Grade:A+</v>
       </c>
       <c r="Q26" s="13"/>
       <c r="R26" s="6" t="str">
         <f>"Range:"&amp;VLOOKUP(D13,'[2]Subject Marks'!$A$3:$BP$122,68,0)</f>
-        <v>Range:65-69.99</v>
+        <v>Range:70.74.99</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
@@ -27930,6 +30244,12 @@
       <c r="S32" s="2"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="9VfSymIJn/CA3Sa6U35zcuAXutJdqD09C4Iv1uzdrxabyyjMra9CY177uWo/Sv+2sDvbjUqAY73j1rPnh3Us1g==" saltValue="QUzrKix66lNFesi3D62EOg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <protectedRanges>
+    <protectedRange sqref="D11" name="Held In"/>
+    <protectedRange sqref="D13" name="Seat No."/>
+    <protectedRange sqref="A27" name="Declared Date"/>
+  </protectedRanges>
   <mergeCells count="39">
     <mergeCell ref="A1:R5"/>
     <mergeCell ref="A7:R7"/>

</xml_diff>